<commit_message>
added predicted Scotland rates pre-1994
</commit_message>
<xml_diff>
--- a/Conception rates by age and country.xlsx
+++ b/Conception rates by age and country.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Under 16" sheetId="1" r:id="rId1"/>
@@ -469,20 +469,107 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -496,95 +583,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2852,633 +2852,666 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG30"/>
+  <dimension ref="A1:AI30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
+        <v>1985</v>
+      </c>
+      <c r="C1">
+        <v>1986</v>
+      </c>
+      <c r="D1">
         <v>1987</v>
       </c>
-      <c r="C1">
-        <f>B1+1</f>
+      <c r="E1">
+        <f>D1+1</f>
         <v>1988</v>
       </c>
-      <c r="D1">
-        <f t="shared" ref="D1:AG1" si="0">C1+1</f>
+      <c r="F1">
+        <f t="shared" ref="F1:AI1" si="0">E1+1</f>
         <v>1989</v>
       </c>
-      <c r="E1">
+      <c r="G1">
         <f t="shared" si="0"/>
         <v>1990</v>
       </c>
-      <c r="F1">
+      <c r="H1">
         <f t="shared" si="0"/>
         <v>1991</v>
       </c>
-      <c r="G1">
+      <c r="I1">
         <f t="shared" si="0"/>
         <v>1992</v>
       </c>
-      <c r="H1">
+      <c r="J1">
         <f t="shared" si="0"/>
         <v>1993</v>
       </c>
-      <c r="I1">
+      <c r="K1">
         <f t="shared" si="0"/>
         <v>1994</v>
       </c>
-      <c r="J1">
+      <c r="L1">
         <f t="shared" si="0"/>
         <v>1995</v>
       </c>
-      <c r="K1">
+      <c r="M1">
         <f t="shared" si="0"/>
         <v>1996</v>
       </c>
-      <c r="L1">
+      <c r="N1">
         <f t="shared" si="0"/>
         <v>1997</v>
       </c>
-      <c r="M1">
+      <c r="O1">
         <f t="shared" si="0"/>
         <v>1998</v>
       </c>
-      <c r="N1">
+      <c r="P1">
         <f t="shared" si="0"/>
         <v>1999</v>
       </c>
-      <c r="O1">
+      <c r="Q1">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="P1">
+      <c r="R1">
         <f t="shared" si="0"/>
         <v>2001</v>
       </c>
-      <c r="Q1">
+      <c r="S1">
         <f t="shared" si="0"/>
         <v>2002</v>
       </c>
-      <c r="R1">
+      <c r="T1">
         <f t="shared" si="0"/>
         <v>2003</v>
       </c>
-      <c r="S1">
+      <c r="U1">
         <f t="shared" si="0"/>
         <v>2004</v>
       </c>
-      <c r="T1">
+      <c r="V1">
         <f t="shared" si="0"/>
         <v>2005</v>
       </c>
-      <c r="U1">
+      <c r="W1">
         <f t="shared" si="0"/>
         <v>2006</v>
       </c>
-      <c r="V1">
+      <c r="X1">
         <f t="shared" si="0"/>
         <v>2007</v>
       </c>
-      <c r="W1">
+      <c r="Y1">
         <f t="shared" si="0"/>
         <v>2008</v>
       </c>
-      <c r="X1">
+      <c r="Z1">
         <f t="shared" si="0"/>
         <v>2009</v>
       </c>
-      <c r="Y1">
+      <c r="AA1">
         <f t="shared" si="0"/>
         <v>2010</v>
       </c>
-      <c r="Z1">
+      <c r="AB1">
         <f t="shared" si="0"/>
         <v>2011</v>
       </c>
-      <c r="AA1">
+      <c r="AC1">
         <f t="shared" si="0"/>
         <v>2012</v>
       </c>
-      <c r="AB1">
-        <f>AA1+1</f>
+      <c r="AD1">
+        <f>AC1+1</f>
         <v>2013</v>
       </c>
-      <c r="AC1">
+      <c r="AE1">
         <f t="shared" si="0"/>
         <v>2014</v>
       </c>
-      <c r="AD1">
+      <c r="AF1">
         <f t="shared" si="0"/>
         <v>2015</v>
       </c>
-      <c r="AE1">
+      <c r="AG1">
         <f t="shared" si="0"/>
         <v>2016</v>
       </c>
-      <c r="AF1">
+      <c r="AH1">
         <f t="shared" si="0"/>
         <v>2017</v>
       </c>
-      <c r="AG1">
+      <c r="AI1">
         <f t="shared" si="0"/>
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="B2" s="2">
+        <v>38.418366115568197</v>
+      </c>
+      <c r="C2" s="2">
+        <v>39.256642256568902</v>
+      </c>
+      <c r="D2" s="2">
+        <v>38.793512380761399</v>
+      </c>
+      <c r="E2" s="2">
+        <v>39.594226250004397</v>
+      </c>
+      <c r="F2" s="2">
+        <v>40.928227491229798</v>
+      </c>
+      <c r="G2" s="2">
+        <v>42.785383249327403</v>
+      </c>
+      <c r="H2" s="2">
+        <v>44.409212627182903</v>
+      </c>
+      <c r="I2" s="2">
+        <v>43.1995217721907</v>
+      </c>
+      <c r="J2" s="2">
+        <v>41.278529201879202</v>
+      </c>
+      <c r="K2">
         <v>41.5</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>40.700000000000003</v>
-      </c>
-      <c r="K2">
-        <v>44.7</v>
-      </c>
-      <c r="L2">
-        <v>43.8</v>
       </c>
       <c r="M2">
         <v>44.7</v>
       </c>
       <c r="N2">
+        <v>43.8</v>
+      </c>
+      <c r="O2">
+        <v>44.7</v>
+      </c>
+      <c r="P2">
         <v>43</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>40.5</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>39.200000000000003</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>39.700000000000003</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>40.200000000000003</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>41.1</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>41.6</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <v>41.2</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>41.9</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <v>40</v>
       </c>
-      <c r="X2">
+      <c r="Z2">
         <v>36.200000000000003</v>
       </c>
-      <c r="Y2">
+      <c r="AA2">
         <v>35.200000000000003</v>
       </c>
-      <c r="Z2">
+      <c r="AB2">
         <v>30</v>
       </c>
-      <c r="AA2">
+      <c r="AC2">
         <v>28</v>
       </c>
-      <c r="AB2">
+      <c r="AD2">
         <v>24.6</v>
       </c>
-      <c r="AC2">
+      <c r="AE2">
         <v>22.1</v>
       </c>
-      <c r="AD2">
+      <c r="AF2">
         <v>20.100000000000001</v>
       </c>
-      <c r="AE2">
+      <c r="AG2">
         <v>18.87</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="D3">
         <v>45.1</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>46.3</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>46.9</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>47.7</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>44.6</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>43.5</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>42.4</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>41.9</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>41.9</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>46.3</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>45.9</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>47.1</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>45.1</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>43.9</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>42.7</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>43</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>42.3</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>41.8</v>
-      </c>
-      <c r="T3">
-        <v>41.6</v>
-      </c>
-      <c r="U3">
-        <v>40.799999999999997</v>
       </c>
       <c r="V3">
         <v>41.6</v>
       </c>
       <c r="W3">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="X3">
+        <v>41.6</v>
+      </c>
+      <c r="Y3">
         <v>39.9</v>
       </c>
-      <c r="X3">
+      <c r="Z3">
         <v>37.200000000000003</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>34.299999999999997</v>
       </c>
-      <c r="Z3">
+      <c r="AB3">
         <v>30.9</v>
       </c>
-      <c r="AA3">
+      <c r="AC3">
         <v>27.9</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <v>24.5</v>
       </c>
-      <c r="AC3">
+      <c r="AE3">
         <v>22.9</v>
       </c>
-      <c r="AD3">
+      <c r="AF3">
         <v>21</v>
       </c>
-      <c r="AE3">
+      <c r="AG3">
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I4" s="1">
         <v>43.3</v>
       </c>
-      <c r="H4" s="2">
+      <c r="J4" s="2">
         <v>42.1</v>
       </c>
-      <c r="I4" s="2">
+      <c r="K4" s="2">
         <v>41.6</v>
       </c>
-      <c r="J4" s="2">
+      <c r="L4" s="2">
         <v>41.6</v>
       </c>
-      <c r="K4" s="2">
+      <c r="M4" s="2">
         <v>45.9</v>
       </c>
-      <c r="L4" s="2">
+      <c r="N4" s="2">
         <v>45.5</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>46.6</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>44.8</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>43.6</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>42.5</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>42.8</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>42.1</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>41.6</v>
-      </c>
-      <c r="T4">
-        <v>41.4</v>
-      </c>
-      <c r="U4">
-        <v>40.6</v>
       </c>
       <c r="V4">
         <v>41.4</v>
       </c>
       <c r="W4">
+        <v>40.6</v>
+      </c>
+      <c r="X4">
+        <v>41.4</v>
+      </c>
+      <c r="Y4">
         <v>39.700000000000003</v>
       </c>
-      <c r="X4">
+      <c r="Z4">
         <v>37.1</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <v>34.200000000000003</v>
       </c>
-      <c r="Z4">
+      <c r="AB4">
         <v>30.7</v>
       </c>
-      <c r="AA4">
+      <c r="AC4">
         <v>27.7</v>
       </c>
-      <c r="AB4">
+      <c r="AD4">
         <v>24.3</v>
       </c>
-      <c r="AC4">
+      <c r="AE4">
         <v>22.8</v>
       </c>
-      <c r="AD4">
+      <c r="AF4">
         <v>20.8</v>
       </c>
-      <c r="AE4">
+      <c r="AG4">
         <v>18.8</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="1">
+      <c r="I5" s="1">
         <v>48</v>
       </c>
-      <c r="H5" s="2">
+      <c r="J5" s="2">
         <v>47.5</v>
       </c>
-      <c r="I5" s="2">
+      <c r="K5" s="2">
         <v>46.4</v>
       </c>
-      <c r="J5" s="2">
+      <c r="L5" s="2">
         <v>48</v>
       </c>
-      <c r="K5" s="2">
+      <c r="M5" s="2">
         <v>53.5</v>
       </c>
-      <c r="L5" s="2">
+      <c r="N5" s="2">
         <v>52.2</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>55</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>51.1</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>48</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>45.5</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>46.2</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>46.1</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>45.5</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>44</v>
       </c>
-      <c r="U5">
+      <c r="W5">
         <v>45.1</v>
       </c>
-      <c r="V5">
+      <c r="X5">
         <v>44.7</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <v>43.7</v>
       </c>
-      <c r="X5">
+      <c r="Z5">
         <v>39.299999999999997</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>36.9</v>
       </c>
-      <c r="Z5">
+      <c r="AB5">
         <v>34.200000000000003</v>
       </c>
-      <c r="AA5">
+      <c r="AC5">
         <v>30.8</v>
       </c>
-      <c r="AB5">
+      <c r="AD5">
         <v>27.3</v>
       </c>
-      <c r="AC5">
+      <c r="AE5">
         <v>25.4</v>
       </c>
-      <c r="AD5">
+      <c r="AF5">
         <v>24.3</v>
       </c>
-      <c r="AE5">
+      <c r="AG5">
         <v>20.9</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="52">
+      <c r="D6" s="52">
         <v>71</v>
       </c>
-      <c r="C6" s="52">
+      <c r="E6" s="52">
         <v>74</v>
       </c>
-      <c r="D6" s="52">
+      <c r="F6" s="52">
         <v>74.8</v>
       </c>
-      <c r="E6" s="52">
+      <c r="G6" s="52">
         <v>74.599999999999994</v>
       </c>
-      <c r="F6" s="52">
+      <c r="H6" s="52">
         <v>73.2</v>
       </c>
-      <c r="G6" s="53">
+      <c r="I6" s="53">
         <v>70.599999999999994</v>
       </c>
-      <c r="H6" s="53">
+      <c r="J6" s="53">
         <v>69.7</v>
       </c>
-      <c r="I6" s="53">
+      <c r="K6" s="53">
         <v>69.099999999999994</v>
       </c>
-      <c r="J6" s="53">
+      <c r="L6" s="53">
         <v>64.400000000000006</v>
       </c>
-      <c r="K6" s="53">
+      <c r="M6" s="53">
         <v>60.7</v>
       </c>
-      <c r="L6" s="53">
+      <c r="N6" s="53">
         <v>56.9</v>
       </c>
-      <c r="M6" s="53">
+      <c r="O6" s="53">
         <v>54.2</v>
       </c>
-      <c r="N6" s="53">
+      <c r="P6" s="53">
         <v>50.8</v>
       </c>
-      <c r="O6" s="53">
+      <c r="Q6" s="53">
         <v>48.4</v>
       </c>
-      <c r="P6" s="53">
+      <c r="R6" s="53">
         <v>44.4</v>
       </c>
-      <c r="Q6" s="53">
+      <c r="S6" s="53">
         <v>42</v>
       </c>
-      <c r="R6" s="53">
+      <c r="T6" s="53">
         <v>40.5</v>
       </c>
-      <c r="S6" s="53">
+      <c r="U6" s="53">
         <v>39.200000000000003</v>
       </c>
-      <c r="T6" s="53">
+      <c r="V6" s="53">
         <v>37.799999999999997</v>
       </c>
-      <c r="U6" s="53">
+      <c r="W6" s="53">
         <v>38.5</v>
       </c>
-      <c r="V6" s="53">
+      <c r="X6" s="53">
         <v>38.1</v>
       </c>
-      <c r="W6" s="53">
+      <c r="Y6" s="53">
         <v>37</v>
       </c>
-      <c r="X6" s="53">
+      <c r="Z6" s="53">
         <v>34.1</v>
       </c>
-      <c r="Y6" s="53">
+      <c r="AA6" s="53">
         <v>30.3</v>
       </c>
-      <c r="Z6" s="53">
+      <c r="AB6" s="53">
         <v>26.7</v>
       </c>
-      <c r="AA6" s="53">
+      <c r="AC6" s="53">
         <v>24</v>
       </c>
-      <c r="AB6" s="53">
+      <c r="AD6" s="53">
         <v>20.8</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="3"/>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="H9:I30">
-    <sortCondition ref="H9:H30"/>
+  <sortState ref="J9:K30">
+    <sortCondition ref="J9:J30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4381,544 +4414,544 @@
       <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="90">
+      <c r="B1" s="64">
         <v>2015</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="89">
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="63">
         <v>2014</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="90">
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="64">
         <v>2013</v>
       </c>
-      <c r="S1" s="90"/>
-      <c r="T1" s="90"/>
-      <c r="U1" s="90"/>
-      <c r="V1" s="90"/>
-      <c r="W1" s="90"/>
-      <c r="X1" s="90"/>
-      <c r="Y1" s="91"/>
-      <c r="Z1" s="89">
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="63">
         <v>2012</v>
       </c>
-      <c r="AA1" s="90"/>
-      <c r="AB1" s="90"/>
-      <c r="AC1" s="90"/>
-      <c r="AD1" s="90"/>
-      <c r="AE1" s="90"/>
-      <c r="AF1" s="90"/>
-      <c r="AG1" s="91"/>
-      <c r="AH1" s="86">
+      <c r="AA1" s="64"/>
+      <c r="AB1" s="64"/>
+      <c r="AC1" s="64"/>
+      <c r="AD1" s="64"/>
+      <c r="AE1" s="64"/>
+      <c r="AF1" s="64"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="75">
         <v>2011</v>
       </c>
-      <c r="AI1" s="87"/>
-      <c r="AJ1" s="87"/>
-      <c r="AK1" s="87"/>
-      <c r="AL1" s="87"/>
-      <c r="AM1" s="87"/>
-      <c r="AN1" s="88"/>
+      <c r="AI1" s="76"/>
+      <c r="AJ1" s="76"/>
+      <c r="AK1" s="76"/>
+      <c r="AL1" s="76"/>
+      <c r="AM1" s="76"/>
+      <c r="AN1" s="77"/>
       <c r="AO1" s="27"/>
-      <c r="AP1" s="86">
+      <c r="AP1" s="75">
         <v>2010</v>
       </c>
-      <c r="AQ1" s="87"/>
-      <c r="AR1" s="87"/>
-      <c r="AS1" s="87"/>
-      <c r="AT1" s="87"/>
-      <c r="AU1" s="87"/>
-      <c r="AV1" s="88"/>
+      <c r="AQ1" s="76"/>
+      <c r="AR1" s="76"/>
+      <c r="AS1" s="76"/>
+      <c r="AT1" s="76"/>
+      <c r="AU1" s="76"/>
+      <c r="AV1" s="77"/>
       <c r="AW1" s="27"/>
-      <c r="AX1" s="89">
+      <c r="AX1" s="63">
         <v>2009</v>
       </c>
-      <c r="AY1" s="90"/>
-      <c r="AZ1" s="90"/>
-      <c r="BA1" s="90"/>
-      <c r="BB1" s="90"/>
-      <c r="BC1" s="90"/>
-      <c r="BD1" s="90"/>
-      <c r="BE1" s="91"/>
+      <c r="AY1" s="64"/>
+      <c r="AZ1" s="64"/>
+      <c r="BA1" s="64"/>
+      <c r="BB1" s="64"/>
+      <c r="BC1" s="64"/>
+      <c r="BD1" s="64"/>
+      <c r="BE1" s="65"/>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="76" t="s">
+      <c r="C2" s="58"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="76" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="74"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="76" t="s">
+      <c r="K2" s="69"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="95"/>
-      <c r="R2" s="78" t="s">
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="74"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="76" t="s">
+      <c r="S2" s="69"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="78"/>
-      <c r="W2" s="78"/>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="84"/>
-      <c r="Z2" s="76" t="s">
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="59"/>
-      <c r="AC2" s="76" t="s">
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="78"/>
-      <c r="AE2" s="78"/>
-      <c r="AF2" s="78"/>
-      <c r="AG2" s="84"/>
-      <c r="AH2" s="76" t="s">
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="59"/>
+      <c r="AH2" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="AI2" s="74"/>
-      <c r="AJ2" s="59"/>
-      <c r="AK2" s="76" t="s">
+      <c r="AI2" s="69"/>
+      <c r="AJ2" s="70"/>
+      <c r="AK2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AL2" s="78"/>
-      <c r="AM2" s="78"/>
-      <c r="AN2" s="78"/>
-      <c r="AO2" s="84"/>
-      <c r="AP2" s="76" t="s">
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="58"/>
+      <c r="AN2" s="58"/>
+      <c r="AO2" s="59"/>
+      <c r="AP2" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="AQ2" s="74"/>
-      <c r="AR2" s="59"/>
-      <c r="AS2" s="76" t="s">
+      <c r="AQ2" s="69"/>
+      <c r="AR2" s="70"/>
+      <c r="AS2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AT2" s="78"/>
-      <c r="AU2" s="78"/>
-      <c r="AV2" s="78"/>
-      <c r="AW2" s="84"/>
-      <c r="AX2" s="76" t="s">
+      <c r="AT2" s="58"/>
+      <c r="AU2" s="58"/>
+      <c r="AV2" s="58"/>
+      <c r="AW2" s="59"/>
+      <c r="AX2" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="74"/>
-      <c r="AZ2" s="59"/>
-      <c r="BA2" s="76" t="s">
+      <c r="AY2" s="69"/>
+      <c r="AZ2" s="70"/>
+      <c r="BA2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="BB2" s="78"/>
-      <c r="BC2" s="78"/>
-      <c r="BD2" s="78"/>
-      <c r="BE2" s="84"/>
+      <c r="BB2" s="58"/>
+      <c r="BC2" s="58"/>
+      <c r="BD2" s="58"/>
+      <c r="BE2" s="59"/>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-      <c r="P3" s="80"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="61"/>
-      <c r="U3" s="82"/>
-      <c r="V3" s="80"/>
-      <c r="W3" s="80"/>
-      <c r="X3" s="80"/>
-      <c r="Y3" s="85"/>
-      <c r="Z3" s="77"/>
-      <c r="AA3" s="73"/>
-      <c r="AB3" s="61"/>
-      <c r="AC3" s="82"/>
-      <c r="AD3" s="80"/>
-      <c r="AE3" s="80"/>
-      <c r="AF3" s="80"/>
-      <c r="AG3" s="85"/>
-      <c r="AH3" s="77"/>
-      <c r="AI3" s="73"/>
-      <c r="AJ3" s="61"/>
-      <c r="AK3" s="82"/>
-      <c r="AL3" s="80"/>
-      <c r="AM3" s="80"/>
-      <c r="AN3" s="80"/>
-      <c r="AO3" s="85"/>
-      <c r="AP3" s="77"/>
-      <c r="AQ3" s="73"/>
-      <c r="AR3" s="61"/>
-      <c r="AS3" s="82"/>
-      <c r="AT3" s="80"/>
-      <c r="AU3" s="80"/>
-      <c r="AV3" s="80"/>
-      <c r="AW3" s="85"/>
-      <c r="AX3" s="77"/>
-      <c r="AY3" s="73"/>
-      <c r="AZ3" s="61"/>
-      <c r="BA3" s="82"/>
-      <c r="BB3" s="80"/>
-      <c r="BC3" s="80"/>
-      <c r="BD3" s="80"/>
-      <c r="BE3" s="85"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="72"/>
+      <c r="S3" s="72"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="61"/>
+      <c r="W3" s="61"/>
+      <c r="X3" s="61"/>
+      <c r="Y3" s="62"/>
+      <c r="Z3" s="71"/>
+      <c r="AA3" s="72"/>
+      <c r="AB3" s="73"/>
+      <c r="AC3" s="60"/>
+      <c r="AD3" s="61"/>
+      <c r="AE3" s="61"/>
+      <c r="AF3" s="61"/>
+      <c r="AG3" s="62"/>
+      <c r="AH3" s="71"/>
+      <c r="AI3" s="72"/>
+      <c r="AJ3" s="73"/>
+      <c r="AK3" s="60"/>
+      <c r="AL3" s="61"/>
+      <c r="AM3" s="61"/>
+      <c r="AN3" s="61"/>
+      <c r="AO3" s="62"/>
+      <c r="AP3" s="71"/>
+      <c r="AQ3" s="72"/>
+      <c r="AR3" s="73"/>
+      <c r="AS3" s="60"/>
+      <c r="AT3" s="61"/>
+      <c r="AU3" s="61"/>
+      <c r="AV3" s="61"/>
+      <c r="AW3" s="62"/>
+      <c r="AX3" s="71"/>
+      <c r="AY3" s="72"/>
+      <c r="AZ3" s="73"/>
+      <c r="BA3" s="60"/>
+      <c r="BB3" s="61"/>
+      <c r="BC3" s="61"/>
+      <c r="BD3" s="61"/>
+      <c r="BE3" s="62"/>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A4" s="93"/>
-      <c r="B4" s="78" t="s">
+      <c r="A4" s="67"/>
+      <c r="B4" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="74" t="s">
+      <c r="C4" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="76" t="s">
+      <c r="E4" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="74" t="s">
+      <c r="F4" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="83"/>
-      <c r="H4" s="74" t="s">
+      <c r="G4" s="85"/>
+      <c r="H4" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="68"/>
-      <c r="J4" s="62" t="s">
+      <c r="I4" s="88"/>
+      <c r="J4" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="65" t="s">
+      <c r="K4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="68" t="s">
+      <c r="L4" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="75" t="s">
+      <c r="M4" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="65" t="s">
+      <c r="N4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="65"/>
-      <c r="P4" s="65" t="s">
+      <c r="O4" s="94"/>
+      <c r="P4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="75" t="s">
+      <c r="Q4" s="70"/>
+      <c r="R4" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="65" t="s">
+      <c r="S4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="68" t="s">
+      <c r="T4" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="75" t="s">
+      <c r="U4" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="V4" s="65" t="s">
+      <c r="V4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="74"/>
-      <c r="X4" s="65" t="s">
+      <c r="W4" s="69"/>
+      <c r="X4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="Y4" s="59"/>
-      <c r="Z4" s="62" t="s">
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="AA4" s="65" t="s">
+      <c r="AA4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="AB4" s="68" t="s">
+      <c r="AB4" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="AC4" s="75" t="s">
+      <c r="AC4" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="AD4" s="65" t="s">
+      <c r="AD4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="AE4" s="74"/>
-      <c r="AF4" s="65" t="s">
+      <c r="AE4" s="69"/>
+      <c r="AF4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="AG4" s="59"/>
-      <c r="AH4" s="75" t="s">
+      <c r="AG4" s="70"/>
+      <c r="AH4" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="AI4" s="65" t="s">
+      <c r="AI4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="68" t="s">
+      <c r="AJ4" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="75" t="s">
+      <c r="AK4" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="AL4" s="65" t="s">
+      <c r="AL4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="AM4" s="74"/>
-      <c r="AN4" s="65" t="s">
+      <c r="AM4" s="69"/>
+      <c r="AN4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="AO4" s="59"/>
-      <c r="AP4" s="75" t="s">
+      <c r="AO4" s="70"/>
+      <c r="AP4" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="AQ4" s="65" t="s">
+      <c r="AQ4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="AR4" s="68" t="s">
+      <c r="AR4" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="AS4" s="75" t="s">
+      <c r="AS4" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="AT4" s="65" t="s">
+      <c r="AT4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="AU4" s="74"/>
-      <c r="AV4" s="65" t="s">
+      <c r="AU4" s="69"/>
+      <c r="AV4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="AW4" s="59"/>
-      <c r="AX4" s="62" t="s">
+      <c r="AW4" s="70"/>
+      <c r="AX4" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="AY4" s="65" t="s">
+      <c r="AY4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="AZ4" s="68" t="s">
+      <c r="AZ4" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="BA4" s="71" t="s">
+      <c r="BA4" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="BB4" s="57" t="s">
+      <c r="BB4" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="BC4" s="72"/>
-      <c r="BD4" s="57" t="s">
+      <c r="BC4" s="82"/>
+      <c r="BD4" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="BE4" s="59"/>
+      <c r="BE4" s="70"/>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A5" s="93"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="57"/>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="57"/>
-      <c r="V5" s="57"/>
-      <c r="W5" s="72"/>
-      <c r="X5" s="57"/>
-      <c r="Y5" s="60"/>
-      <c r="Z5" s="63"/>
-      <c r="AA5" s="66"/>
-      <c r="AB5" s="69"/>
-      <c r="AC5" s="57"/>
-      <c r="AD5" s="57"/>
-      <c r="AE5" s="72"/>
-      <c r="AF5" s="57"/>
-      <c r="AG5" s="60"/>
-      <c r="AH5" s="57"/>
-      <c r="AI5" s="66"/>
-      <c r="AJ5" s="69"/>
-      <c r="AK5" s="57"/>
-      <c r="AL5" s="66"/>
-      <c r="AM5" s="72"/>
-      <c r="AN5" s="57"/>
-      <c r="AO5" s="60"/>
-      <c r="AP5" s="57"/>
-      <c r="AQ5" s="66"/>
-      <c r="AR5" s="69"/>
-      <c r="AS5" s="57"/>
-      <c r="AT5" s="66"/>
-      <c r="AU5" s="72"/>
-      <c r="AV5" s="57"/>
-      <c r="AW5" s="60"/>
-      <c r="AX5" s="63"/>
-      <c r="AY5" s="66"/>
-      <c r="AZ5" s="69"/>
-      <c r="BA5" s="57"/>
-      <c r="BB5" s="66"/>
-      <c r="BC5" s="72"/>
-      <c r="BD5" s="57"/>
-      <c r="BE5" s="60"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="89"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="83"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="89"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="79"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="79"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="92"/>
+      <c r="AA5" s="86"/>
+      <c r="AB5" s="89"/>
+      <c r="AC5" s="79"/>
+      <c r="AD5" s="79"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="79"/>
+      <c r="AG5" s="83"/>
+      <c r="AH5" s="79"/>
+      <c r="AI5" s="86"/>
+      <c r="AJ5" s="89"/>
+      <c r="AK5" s="79"/>
+      <c r="AL5" s="86"/>
+      <c r="AM5" s="82"/>
+      <c r="AN5" s="79"/>
+      <c r="AO5" s="83"/>
+      <c r="AP5" s="79"/>
+      <c r="AQ5" s="86"/>
+      <c r="AR5" s="89"/>
+      <c r="AS5" s="79"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="82"/>
+      <c r="AV5" s="79"/>
+      <c r="AW5" s="83"/>
+      <c r="AX5" s="92"/>
+      <c r="AY5" s="86"/>
+      <c r="AZ5" s="89"/>
+      <c r="BA5" s="79"/>
+      <c r="BB5" s="86"/>
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="79"/>
+      <c r="BE5" s="83"/>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A6" s="93"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57"/>
-      <c r="O6" s="57"/>
-      <c r="P6" s="57"/>
-      <c r="Q6" s="60"/>
-      <c r="R6" s="57"/>
-      <c r="S6" s="66"/>
-      <c r="T6" s="69"/>
-      <c r="U6" s="57"/>
-      <c r="V6" s="57"/>
-      <c r="W6" s="72"/>
-      <c r="X6" s="57"/>
-      <c r="Y6" s="60"/>
-      <c r="Z6" s="63"/>
-      <c r="AA6" s="66"/>
-      <c r="AB6" s="69"/>
-      <c r="AC6" s="57"/>
-      <c r="AD6" s="57"/>
-      <c r="AE6" s="72"/>
-      <c r="AF6" s="57"/>
-      <c r="AG6" s="60"/>
-      <c r="AH6" s="57"/>
-      <c r="AI6" s="66"/>
-      <c r="AJ6" s="69"/>
-      <c r="AK6" s="57"/>
-      <c r="AL6" s="66"/>
-      <c r="AM6" s="72"/>
-      <c r="AN6" s="57"/>
-      <c r="AO6" s="60"/>
-      <c r="AP6" s="57"/>
-      <c r="AQ6" s="66"/>
-      <c r="AR6" s="69"/>
-      <c r="AS6" s="57"/>
-      <c r="AT6" s="66"/>
-      <c r="AU6" s="72"/>
-      <c r="AV6" s="57"/>
-      <c r="AW6" s="60"/>
-      <c r="AX6" s="63"/>
-      <c r="AY6" s="66"/>
-      <c r="AZ6" s="69"/>
-      <c r="BA6" s="57"/>
-      <c r="BB6" s="66"/>
-      <c r="BC6" s="72"/>
-      <c r="BD6" s="57"/>
-      <c r="BE6" s="60"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="79"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="83"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="86"/>
+      <c r="T6" s="89"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="82"/>
+      <c r="X6" s="79"/>
+      <c r="Y6" s="83"/>
+      <c r="Z6" s="92"/>
+      <c r="AA6" s="86"/>
+      <c r="AB6" s="89"/>
+      <c r="AC6" s="79"/>
+      <c r="AD6" s="79"/>
+      <c r="AE6" s="82"/>
+      <c r="AF6" s="79"/>
+      <c r="AG6" s="83"/>
+      <c r="AH6" s="79"/>
+      <c r="AI6" s="86"/>
+      <c r="AJ6" s="89"/>
+      <c r="AK6" s="79"/>
+      <c r="AL6" s="86"/>
+      <c r="AM6" s="82"/>
+      <c r="AN6" s="79"/>
+      <c r="AO6" s="83"/>
+      <c r="AP6" s="79"/>
+      <c r="AQ6" s="86"/>
+      <c r="AR6" s="89"/>
+      <c r="AS6" s="79"/>
+      <c r="AT6" s="86"/>
+      <c r="AU6" s="82"/>
+      <c r="AV6" s="79"/>
+      <c r="AW6" s="83"/>
+      <c r="AX6" s="92"/>
+      <c r="AY6" s="86"/>
+      <c r="AZ6" s="89"/>
+      <c r="BA6" s="79"/>
+      <c r="BB6" s="86"/>
+      <c r="BC6" s="82"/>
+      <c r="BD6" s="79"/>
+      <c r="BE6" s="83"/>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A7" s="94"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="61"/>
-      <c r="R7" s="58"/>
-      <c r="S7" s="67"/>
-      <c r="T7" s="70"/>
-      <c r="U7" s="58"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="73"/>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="61"/>
-      <c r="Z7" s="64"/>
-      <c r="AA7" s="67"/>
-      <c r="AB7" s="70"/>
-      <c r="AC7" s="58"/>
-      <c r="AD7" s="58"/>
-      <c r="AE7" s="73"/>
-      <c r="AF7" s="58"/>
-      <c r="AG7" s="61"/>
-      <c r="AH7" s="58"/>
-      <c r="AI7" s="67"/>
-      <c r="AJ7" s="70"/>
-      <c r="AK7" s="58"/>
-      <c r="AL7" s="67"/>
-      <c r="AM7" s="73"/>
-      <c r="AN7" s="58"/>
-      <c r="AO7" s="61"/>
-      <c r="AP7" s="58"/>
-      <c r="AQ7" s="67"/>
-      <c r="AR7" s="70"/>
-      <c r="AS7" s="58"/>
-      <c r="AT7" s="67"/>
-      <c r="AU7" s="73"/>
-      <c r="AV7" s="58"/>
-      <c r="AW7" s="61"/>
-      <c r="AX7" s="64"/>
-      <c r="AY7" s="67"/>
-      <c r="AZ7" s="70"/>
-      <c r="BA7" s="58"/>
-      <c r="BB7" s="67"/>
-      <c r="BC7" s="73"/>
-      <c r="BD7" s="58"/>
-      <c r="BE7" s="61"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="90"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="80"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="80"/>
+      <c r="S7" s="87"/>
+      <c r="T7" s="90"/>
+      <c r="U7" s="80"/>
+      <c r="V7" s="80"/>
+      <c r="W7" s="72"/>
+      <c r="X7" s="80"/>
+      <c r="Y7" s="73"/>
+      <c r="Z7" s="93"/>
+      <c r="AA7" s="87"/>
+      <c r="AB7" s="90"/>
+      <c r="AC7" s="80"/>
+      <c r="AD7" s="80"/>
+      <c r="AE7" s="72"/>
+      <c r="AF7" s="80"/>
+      <c r="AG7" s="73"/>
+      <c r="AH7" s="80"/>
+      <c r="AI7" s="87"/>
+      <c r="AJ7" s="90"/>
+      <c r="AK7" s="80"/>
+      <c r="AL7" s="87"/>
+      <c r="AM7" s="72"/>
+      <c r="AN7" s="80"/>
+      <c r="AO7" s="73"/>
+      <c r="AP7" s="80"/>
+      <c r="AQ7" s="87"/>
+      <c r="AR7" s="90"/>
+      <c r="AS7" s="80"/>
+      <c r="AT7" s="87"/>
+      <c r="AU7" s="72"/>
+      <c r="AV7" s="80"/>
+      <c r="AW7" s="73"/>
+      <c r="AX7" s="93"/>
+      <c r="AY7" s="87"/>
+      <c r="AZ7" s="90"/>
+      <c r="BA7" s="80"/>
+      <c r="BB7" s="87"/>
+      <c r="BC7" s="72"/>
+      <c r="BD7" s="80"/>
+      <c r="BE7" s="73"/>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
@@ -5799,6 +5832,68 @@
     <sortCondition descending="1" ref="K23"/>
   </sortState>
   <mergeCells count="78">
+    <mergeCell ref="BD4:BD7"/>
+    <mergeCell ref="BE4:BE7"/>
+    <mergeCell ref="AX4:AX7"/>
+    <mergeCell ref="AY4:AY7"/>
+    <mergeCell ref="AZ4:AZ7"/>
+    <mergeCell ref="BA4:BA7"/>
+    <mergeCell ref="BB4:BB7"/>
+    <mergeCell ref="BC4:BC7"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="AL4:AL7"/>
+    <mergeCell ref="AM4:AM7"/>
+    <mergeCell ref="AN4:AN7"/>
+    <mergeCell ref="AO4:AO7"/>
+    <mergeCell ref="AP4:AP7"/>
+    <mergeCell ref="AQ4:AQ7"/>
+    <mergeCell ref="AR4:AR7"/>
+    <mergeCell ref="AS4:AS7"/>
+    <mergeCell ref="AT4:AT7"/>
+    <mergeCell ref="AU4:AU7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="U4:U7"/>
+    <mergeCell ref="V4:V7"/>
+    <mergeCell ref="W4:W7"/>
+    <mergeCell ref="X4:X7"/>
+    <mergeCell ref="AK4:AK7"/>
+    <mergeCell ref="Z4:Z7"/>
+    <mergeCell ref="AA4:AA7"/>
+    <mergeCell ref="AB4:AB7"/>
+    <mergeCell ref="AC4:AC7"/>
+    <mergeCell ref="AD4:AD7"/>
+    <mergeCell ref="AE4:AE7"/>
+    <mergeCell ref="AF4:AF7"/>
+    <mergeCell ref="AG4:AG7"/>
+    <mergeCell ref="AH4:AH7"/>
+    <mergeCell ref="AI4:AI7"/>
+    <mergeCell ref="AJ4:AJ7"/>
+    <mergeCell ref="P4:P7"/>
+    <mergeCell ref="Q4:Q7"/>
+    <mergeCell ref="R4:R7"/>
+    <mergeCell ref="S4:S7"/>
+    <mergeCell ref="T4:T7"/>
+    <mergeCell ref="AX2:AZ3"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="Y4:Y7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="O4:O7"/>
+    <mergeCell ref="AH2:AJ3"/>
+    <mergeCell ref="AK2:AO3"/>
+    <mergeCell ref="AP2:AR3"/>
+    <mergeCell ref="AS2:AW3"/>
+    <mergeCell ref="AP1:AV1"/>
     <mergeCell ref="BA2:BE3"/>
     <mergeCell ref="AX1:BE1"/>
     <mergeCell ref="A2:A7"/>
@@ -5815,68 +5910,6 @@
     <mergeCell ref="R1:Y1"/>
     <mergeCell ref="Z1:AG1"/>
     <mergeCell ref="AH1:AN1"/>
-    <mergeCell ref="AH2:AJ3"/>
-    <mergeCell ref="AK2:AO3"/>
-    <mergeCell ref="AP2:AR3"/>
-    <mergeCell ref="AS2:AW3"/>
-    <mergeCell ref="AP1:AV1"/>
-    <mergeCell ref="AX2:AZ3"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="Y4:Y7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="O4:O7"/>
-    <mergeCell ref="P4:P7"/>
-    <mergeCell ref="Q4:Q7"/>
-    <mergeCell ref="R4:R7"/>
-    <mergeCell ref="S4:S7"/>
-    <mergeCell ref="T4:T7"/>
-    <mergeCell ref="U4:U7"/>
-    <mergeCell ref="V4:V7"/>
-    <mergeCell ref="W4:W7"/>
-    <mergeCell ref="X4:X7"/>
-    <mergeCell ref="AK4:AK7"/>
-    <mergeCell ref="Z4:Z7"/>
-    <mergeCell ref="AA4:AA7"/>
-    <mergeCell ref="AB4:AB7"/>
-    <mergeCell ref="AC4:AC7"/>
-    <mergeCell ref="AD4:AD7"/>
-    <mergeCell ref="AE4:AE7"/>
-    <mergeCell ref="AF4:AF7"/>
-    <mergeCell ref="AG4:AG7"/>
-    <mergeCell ref="AH4:AH7"/>
-    <mergeCell ref="AI4:AI7"/>
-    <mergeCell ref="AJ4:AJ7"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="AL4:AL7"/>
-    <mergeCell ref="AM4:AM7"/>
-    <mergeCell ref="AN4:AN7"/>
-    <mergeCell ref="AO4:AO7"/>
-    <mergeCell ref="AP4:AP7"/>
-    <mergeCell ref="AQ4:AQ7"/>
-    <mergeCell ref="AR4:AR7"/>
-    <mergeCell ref="AS4:AS7"/>
-    <mergeCell ref="AT4:AT7"/>
-    <mergeCell ref="AU4:AU7"/>
-    <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="BD4:BD7"/>
-    <mergeCell ref="BE4:BE7"/>
-    <mergeCell ref="AX4:AX7"/>
-    <mergeCell ref="AY4:AY7"/>
-    <mergeCell ref="AZ4:AZ7"/>
-    <mergeCell ref="BA4:BA7"/>
-    <mergeCell ref="BB4:BB7"/>
-    <mergeCell ref="BC4:BC7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5886,7 +5919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>